<commit_message>
Changes to poaching cost parameter, w.
</commit_message>
<xml_diff>
--- a/data/c_par.xlsx
+++ b/data/c_par.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmlawson/github/totoaba/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD5958F-6934-874D-9550-D08A46E1C610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDA69E7-E851-9E46-8347-CE2087694730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="680" windowWidth="27640" windowHeight="10680" xr2:uid="{A9F12E21-E1E7-D945-BD15-FB70EC07F795}"/>
+    <workbookView xWindow="5900" yWindow="1840" windowWidth="27640" windowHeight="10680" xr2:uid="{A9F12E21-E1E7-D945-BD15-FB70EC07F795}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,9 +53,6 @@
     <t>totoaba_t_per_vessel</t>
   </si>
   <si>
-    <t>price_poachers_per_t</t>
-  </si>
-  <si>
     <t>vesseldays_month</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>vessel_cost</t>
+  </si>
+  <si>
+    <t>price_poachers_per_totoaba</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,31 +454,31 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -498,7 +498,7 @@
         <v>0.8</v>
       </c>
       <c r="F2">
-        <v>34595.33</v>
+        <v>16045</v>
       </c>
       <c r="G2">
         <f>B2*C2</f>
@@ -544,7 +544,7 @@
         <v>4.95</v>
       </c>
       <c r="F3">
-        <v>34595.33</v>
+        <v>16045</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G13" si="0">B3*C3</f>
@@ -590,7 +590,7 @@
         <v>9.8800000000000008</v>
       </c>
       <c r="F4">
-        <v>34595.33</v>
+        <v>16045</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -636,7 +636,7 @@
         <v>13.16</v>
       </c>
       <c r="F5">
-        <v>34595.33</v>
+        <v>16045</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -682,7 +682,7 @@
         <v>4.95</v>
       </c>
       <c r="F6">
-        <v>34595.33</v>
+        <v>16045</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -728,7 +728,7 @@
         <v>0.8</v>
       </c>
       <c r="F7">
-        <v>34595.33</v>
+        <v>16045</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Minor changes to data files
</commit_message>
<xml_diff>
--- a/data/c_par.xlsx
+++ b/data/c_par.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmlawson/github/totoaba/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB05F66-ACBA-4045-BFCD-714049FFEFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAB1732-A9E5-4841-A750-8FAA54678C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="10080" windowWidth="21340" windowHeight="12600" xr2:uid="{A9F12E21-E1E7-D945-BD15-FB70EC07F795}"/>
+    <workbookView xWindow="2840" yWindow="5980" windowWidth="33580" windowHeight="16700" xr2:uid="{A9F12E21-E1E7-D945-BD15-FB70EC07F795}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>